<commit_message>
Update Uganda transformation scenario Excel file with new data
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_uganda_transformation_cw_bau.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_uganda_transformation_cw_bau.xlsx
@@ -1561,12 +1561,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1575,6 +1569,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFff0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1692,7 +1692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1721,94 +1721,94 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -1817,16 +1817,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2160,27 +2157,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="46" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="46" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="46" width="43.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="46" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="46" width="62.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="46" width="33.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="47" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="46" width="47.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="46" width="48.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="46" width="40.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="46" width="35.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="46" width="35.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="48" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="49" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="49" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="49" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="49" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="50" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="51" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="49" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="52" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="45" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="45" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="45" width="43.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="45" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="45" width="62.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="45" width="33.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="46" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="45" width="47.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="45" width="48.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="45" width="40.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="45" width="35.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="45" width="35.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="47" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="48" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="48" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="48" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="48" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="49" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="50" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="48" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="51" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="65.1" customFormat="1" s="4">
@@ -2240,7 +2237,7 @@
       <c r="T1" s="11"/>
       <c r="U1" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="162.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="154.5" customFormat="1" s="4">
       <c r="A2" s="12" t="s">
         <v>217</v>
       </c>
@@ -2291,7 +2288,7 @@
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A3" s="12" t="s">
         <v>217</v>
       </c>
@@ -2334,7 +2331,7 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="48.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="46.5" customFormat="1" s="4">
       <c r="A4" s="12" t="s">
         <v>217</v>
       </c>
@@ -2377,7 +2374,7 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="105.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="100.5" customFormat="1" s="4">
       <c r="A5" s="12" t="s">
         <v>217</v>
       </c>
@@ -2426,7 +2423,7 @@
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="162.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="154.5" customFormat="1" s="4">
       <c r="A6" s="12" t="s">
         <v>217</v>
       </c>
@@ -2483,7 +2480,7 @@
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="48.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="46.5" customFormat="1" s="4">
       <c r="A7" s="25" t="s">
         <v>239</v>
       </c>
@@ -5300,7 +5297,7 @@
       <c r="P63" s="36"/>
       <c r="Q63" s="36"/>
       <c r="R63" s="38"/>
-      <c r="S63" s="44"/>
+      <c r="S63" s="38"/>
       <c r="T63" s="36"/>
       <c r="U63" s="37"/>
     </row>
@@ -5323,7 +5320,7 @@
       <c r="P64" s="36"/>
       <c r="Q64" s="36"/>
       <c r="R64" s="38"/>
-      <c r="S64" s="44"/>
+      <c r="S64" s="38"/>
       <c r="T64" s="36"/>
       <c r="U64" s="37"/>
     </row>
@@ -5345,8 +5342,8 @@
       <c r="O65" s="36"/>
       <c r="P65" s="36"/>
       <c r="Q65" s="36"/>
-      <c r="R65" s="45"/>
-      <c r="S65" s="44"/>
+      <c r="R65" s="44"/>
+      <c r="S65" s="38"/>
       <c r="T65" s="36"/>
       <c r="U65" s="35"/>
     </row>

</xml_diff>